<commit_message>
updated data files and added harvest plots to vis_to_file.py
</commit_message>
<xml_diff>
--- a/data/figs/projects/projects.xlsx
+++ b/data/figs/projects/projects.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="56">
   <si>
     <t>Apr-2019</t>
   </si>
@@ -100,31 +100,37 @@
     <t>Parallel Monte Carlo</t>
   </si>
   <si>
+    <t>Probabilistic FEM</t>
+  </si>
+  <si>
     <t>Streaming healthcare analytics</t>
   </si>
   <si>
     <t>Team management</t>
   </si>
   <si>
+    <t>UQM^3</t>
+  </si>
+  <si>
     <t>Uncertainty in Government Modelling</t>
   </si>
   <si>
     <t>Urban observatory spatial sampling</t>
   </si>
   <si>
-    <t>May Yong (0.5)</t>
-  </si>
-  <si>
-    <t>Louise Bowler (0.5)</t>
-  </si>
-  <si>
-    <t>Sarah Gibson (0.5)</t>
-  </si>
-  <si>
-    <t>Radka Jersakova (0.5)</t>
-  </si>
-  <si>
-    <t>Tomas Lazauskas (0.5)</t>
+    <t>May Yong (0.6)</t>
+  </si>
+  <si>
+    <t>Louise Bowler (0.6)</t>
+  </si>
+  <si>
+    <t>Sarah Gibson (0.6)</t>
+  </si>
+  <si>
+    <t>Radka Jersakova (0.6)</t>
+  </si>
+  <si>
+    <t>Tomas Lazauskas (0.6)</t>
   </si>
   <si>
     <t>Miguel Morin (0.6)</t>
@@ -133,58 +139,49 @@
     <t>Evelina Gabasova (0.6)</t>
   </si>
   <si>
-    <t>Giovanni Colavizza (0.2)</t>
-  </si>
-  <si>
-    <t>James Robinson (0.5)</t>
-  </si>
-  <si>
-    <t>Nick Barlow (0.5)</t>
-  </si>
-  <si>
-    <t>Miguel Morin (0.5)</t>
-  </si>
-  <si>
-    <t>Evelina Gabasova (0.5)</t>
-  </si>
-  <si>
-    <t>Jim Madge (0.5)</t>
-  </si>
-  <si>
-    <t>Camila Rangel Smith (0.5)</t>
+    <t>Giovanni Colavizza (0.3)</t>
+  </si>
+  <si>
+    <t>James Robinson (0.6)</t>
+  </si>
+  <si>
+    <t>Nick Barlow (0.6)</t>
+  </si>
+  <si>
+    <t>Jim Madge (0.6)</t>
+  </si>
+  <si>
+    <t>Camila Rangel Smith (0.6)</t>
   </si>
   <si>
     <t>RESOURCE REQUIRED (0.6)</t>
   </si>
   <si>
-    <t>Louise Bowler (0.6)</t>
-  </si>
-  <si>
-    <t>David Beavan (1.0)</t>
-  </si>
-  <si>
-    <t>Timothy Hobson (0.5)</t>
-  </si>
-  <si>
-    <t>Giovanni Colavizza (0.5)</t>
+    <t>David Beavan (1.2)</t>
+  </si>
+  <si>
+    <t>Timothy Hobson (0.6)</t>
+  </si>
+  <si>
+    <t>Giovanni Colavizza (0.6)</t>
   </si>
   <si>
     <t>James Hetherington (0.1)</t>
   </si>
   <si>
+    <t>James Geddes (0.6)</t>
+  </si>
+  <si>
     <t>Oliver Strickson (0.6)</t>
   </si>
   <si>
-    <t>James Geddes (0.5)</t>
-  </si>
-  <si>
-    <t>Camila Rangel Smith (0.6)</t>
+    <t>Eric Daub (0.6)</t>
+  </si>
+  <si>
+    <t>Eric Daub (0.5)</t>
   </si>
   <si>
     <t>RESOURCE REQUIRED (0.5)</t>
-  </si>
-  <si>
-    <t>James Robinson (0.4)</t>
   </si>
 </sst>
 </file>
@@ -215,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,7 +221,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF84B17A"/>
+        <fgColor rgb="FFD481C2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,13 +233,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4FAE5"/>
+        <fgColor rgb="FFB2FD8B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA6EC84"/>
+        <fgColor rgb="FFFC92EA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,85 +251,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCFD2B4"/>
+        <fgColor rgb="FF85E981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7CECB9"/>
+        <fgColor rgb="FFA495F8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF686"/>
+        <fgColor rgb="FFFFE48E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2A5C3"/>
+        <fgColor rgb="FF7F80C4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7EF7FF"/>
+        <fgColor rgb="FF88F3F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF67BF7"/>
+        <fgColor rgb="FFFD837D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF94B5D2"/>
+        <fgColor rgb="FF94CDBF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFABF1CC"/>
+        <fgColor rgb="FFF5ACAD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCB9B9B"/>
+        <fgColor rgb="FFD0FEBE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBADAF7"/>
+        <fgColor rgb="FF8F927F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA07A8C"/>
+        <fgColor rgb="FFFEF8EC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFB8C81"/>
+        <fgColor rgb="FFC9C2CA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7F8CB3"/>
+        <fgColor rgb="FF82AFA6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEAC68D"/>
+        <fgColor rgb="FFCF9385"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDED1FC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -424,6 +427,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -720,7 +726,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -775,10 +781,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -798,10 +804,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -823,25 +829,25 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>55</v>
@@ -860,25 +866,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -895,28 +901,28 @@
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -932,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>46</v>
@@ -975,40 +981,40 @@
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O8" s="3"/>
     </row>
@@ -1020,31 +1026,31 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1059,31 +1065,31 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1098,31 +1104,31 @@
         <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1137,40 +1143,40 @@
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O12" s="3"/>
     </row>
@@ -1180,10 +1186,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1310,43 +1316,43 @@
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1357,43 +1363,43 @@
         <v>1</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1402,43 +1408,43 @@
         <v>2</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1447,40 +1453,40 @@
         <v>3</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M20" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O20" s="3"/>
     </row>
@@ -1490,31 +1496,31 @@
         <v>4</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1529,31 +1535,31 @@
         <v>1</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1566,31 +1572,31 @@
         <v>2</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -1603,31 +1609,31 @@
         <v>3</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1642,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1665,10 +1671,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1690,10 +1696,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1714,33 +1720,21 @@
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="C28" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
@@ -1753,32 +1747,32 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="K29" s="18" t="s">
-        <v>51</v>
+      <c r="C29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -1792,42 +1786,36 @@
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="M30" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N30" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="C30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
     <row r="31" spans="1:15">
@@ -1837,37 +1825,109 @@
       <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="C31" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>